<commit_message>
create import xlsx system for vendor
</commit_message>
<xml_diff>
--- a/public/files/example-vendors-csv.xlsx
+++ b/public/files/example-vendors-csv.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="43">
   <si>
     <t xml:space="preserve">Name</t>
   </si>
@@ -53,6 +53,166 @@
   </si>
   <si>
     <t xml:space="preserve">GSTIN Number</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">mono </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">ranjan</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">mono@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mr mono</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bangladesh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dhaka</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tongi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">address, address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">web developer</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">shumon </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">babu</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">shumon@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mr mauro</t>
+  </si>
+  <si>
+    <t xml:space="preserve">india</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gazipur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">habiganj</t>
+  </si>
+  <si>
+    <t xml:space="preserve">address2, address2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dev ops</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">shakhor </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">das</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">shakhor@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mr shuja</t>
+  </si>
+  <si>
+    <t xml:space="preserve">italy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sylhet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kishorganj</t>
+  </si>
+  <si>
+    <t xml:space="preserve">address3, address3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">designer</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">samir </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="0"/>
+      </rPr>
+      <t xml:space="preserve">developer</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">samir@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mr samir</t>
+  </si>
+  <si>
+    <t xml:space="preserve">london</t>
+  </si>
+  <si>
+    <t xml:space="preserve">england</t>
+  </si>
+  <si>
+    <t xml:space="preserve">the new city</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Address4, address4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">learner</t>
   </si>
 </sst>
 </file>
@@ -63,7 +223,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -88,6 +248,24 @@
     <font>
       <b val="true"/>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <family val="0"/>
       <charset val="1"/>
@@ -135,24 +313,32 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -176,12 +362,12 @@
   <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
+      <selection pane="topLeft" activeCell="K5" activeCellId="0" sqref="K5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5078125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="9.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="17.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="16.2"/>
@@ -194,65 +380,187 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="17.42"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="K2" s="3" t="s">
-        <v>10</v>
+    <row r="2" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>1522</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>1230</v>
+      </c>
+      <c r="I2" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="K2" s="5" t="n">
+        <v>20</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D3" s="4"/>
+    <row r="3" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>1749</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="H3" s="0" t="n">
+        <v>3360</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="K3" s="0" t="n">
+        <v>54</v>
+      </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D4" s="4"/>
+    <row r="4" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>32155</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="H4" s="0" t="n">
+        <v>1219</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="K4" s="0" t="n">
+        <v>254</v>
+      </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D5" s="4"/>
+    <row r="5" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>543521</v>
+      </c>
+      <c r="D5" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>4152</v>
+      </c>
+      <c r="I5" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="K5" s="0" t="n">
+        <v>41</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:I1"/>
-  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" display="mono@gmail.com"/>
+    <hyperlink ref="B4" r:id="rId2" display="shakhor@gmail.com"/>
+    <hyperlink ref="B5" r:id="rId3" display="samir@gmail.com"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>